<commit_message>
Change to bi-directional logic level shifter - works.
</commit_message>
<xml_diff>
--- a/PCB-shield/REV2-BOM.xlsx
+++ b/PCB-shield/REV2-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AOM\IoT-Bit\AoM-IoT-Bit\PCB-shield\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marka\AoM\IoT-Bit\AoM-IoT-Bit\PCB-shield\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B06F26-8B74-4F59-AEED-E1D0E6DCBC52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B949DEFD-8D85-4663-A24A-64EFBF3D6506}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="53">
   <si>
     <t>Name/Desc</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>Assembly Total Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x14-pin long male headers </t>
+  </si>
+  <si>
+    <t>https://www.adafruit.com/product/392</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1x3-pin long male headers </t>
   </si>
 </sst>
 </file>
@@ -311,10 +320,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -335,7 +341,10 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -620,10 +629,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="H21" sqref="H21:H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,81 +645,81 @@
     <col min="6" max="6" width="7.88671875" style="3" customWidth="1"/>
     <col min="7" max="7" width="37.5546875" style="1" customWidth="1"/>
     <col min="8" max="8" width="10.6640625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="19.33203125" style="15" customWidth="1"/>
-    <col min="11" max="11" width="11.77734375" style="15" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="5" customWidth="1"/>
+    <col min="11" max="11" width="11.77734375" style="5" customWidth="1"/>
     <col min="12" max="12" width="16.6640625" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="13" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10"/>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="12" t="s">
+      <c r="H1" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="14" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7" t="s">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>1</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="8">
         <v>2.08</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="8">
         <f>PRODUCT(E2*F2)</f>
         <v>2.08</v>
       </c>
       <c r="I2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="14">
+      <c r="J2" s="13">
         <f>SUM(H1:H100)</f>
-        <v>9.5900000000000016</v>
-      </c>
-      <c r="K2" s="8">
+        <v>10.090000000000002</v>
+      </c>
+      <c r="K2" s="7">
         <v>4</v>
       </c>
-      <c r="L2" s="8">
+      <c r="L2" s="13">
         <f>PRODUCT(J2, K2)</f>
-        <v>38.360000000000007</v>
+        <v>40.360000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -733,13 +742,12 @@
         <v>8</v>
       </c>
       <c r="H3" s="3">
-        <f t="shared" ref="H3:H18" si="0">PRODUCT(E3*F3)</f>
+        <f t="shared" ref="H3:H28" si="0">PRODUCT(E3*F3)</f>
         <v>0.38</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
@@ -767,7 +775,6 @@
       <c r="I4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
@@ -795,7 +802,6 @@
       <c r="I5" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
@@ -823,7 +829,6 @@
       <c r="I6" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
@@ -851,7 +856,6 @@
       <c r="I7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
@@ -879,7 +883,6 @@
       <c r="I8" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B9" s="1" t="s">
@@ -907,7 +910,6 @@
       <c r="I9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -935,7 +937,6 @@
       <c r="I10" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
@@ -963,7 +964,6 @@
       <c r="I11" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
@@ -990,7 +990,6 @@
       <c r="I12" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
@@ -1017,7 +1016,6 @@
       <c r="I13" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
@@ -1044,7 +1042,6 @@
       <c r="I14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
@@ -1071,7 +1068,6 @@
       <c r="I15" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B16" s="1" t="s">
@@ -1098,7 +1094,6 @@
       <c r="I16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
@@ -1145,6 +1140,54 @@
       <c r="H18" s="3">
         <f t="shared" si="0"/>
         <v>1.07</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="2">
+        <v>392</v>
+      </c>
+      <c r="E19" s="2">
+        <v>2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="2">
+        <v>392</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1</v>
+      </c>
+      <c r="F20" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>